<commit_message>
some corrections in the 24Spkxcel file
</commit_message>
<xml_diff>
--- a/data/figSup34Spk.xlsx
+++ b/data/figSup34Spk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\travail\sourcecode\developing\paper\centriG\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdesbois/pg/chrisPg/centriG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82749739-FECF-465C-A50B-10B5588042D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033B6656-8A2B-BC49-ACCD-FCF2CE2520AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -357,9 +351,6 @@
     <t>vmsrndIsoStcDgain50Indisig</t>
   </si>
   <si>
-    <t>vmfrnIsodStcDlat50</t>
-  </si>
-  <si>
     <t>vmfrndIsoStcDlat50Indisig</t>
   </si>
   <si>
@@ -994,13 +985,16 @@
   </si>
   <si>
     <t>vmsrndIsoStcDlat50</t>
+  </si>
+  <si>
+    <t>vmfrndIsoStcDlat50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1049,7 +1043,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1348,32 +1342,32 @@
   <dimension ref="A1:AG21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z1" sqref="Z1:Z1048576"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="9" width="27.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="9" width="27.5" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" customWidth="1"/>
     <col min="11" max="11" width="28" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="17" width="29.28515625" customWidth="1"/>
-    <col min="18" max="18" width="26.5703125" customWidth="1"/>
+    <col min="13" max="17" width="29.33203125" customWidth="1"/>
+    <col min="18" max="18" width="26.5" customWidth="1"/>
     <col min="19" max="25" width="29" customWidth="1"/>
     <col min="26" max="26" width="23" customWidth="1"/>
-    <col min="27" max="27" width="32.85546875" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" customWidth="1"/>
-    <col min="29" max="33" width="29.5703125" customWidth="1"/>
-    <col min="34" max="34" width="27.85546875" customWidth="1"/>
-    <col min="35" max="35" width="31.140625" customWidth="1"/>
+    <col min="27" max="27" width="32.83203125" customWidth="1"/>
+    <col min="28" max="28" width="26.1640625" customWidth="1"/>
+    <col min="29" max="33" width="29.5" customWidth="1"/>
+    <col min="34" max="34" width="27.83203125" customWidth="1"/>
+    <col min="35" max="35" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1450,7 +1444,7 @@
         <v>44</v>
       </c>
       <c r="Z1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AA1" t="s">
         <v>105</v>
@@ -1462,30 +1456,30 @@
         <v>107</v>
       </c>
       <c r="AD1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AE1" t="s">
         <v>108</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>109</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>110</v>
       </c>
-      <c r="AG1" t="s">
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1497,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1509,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1521,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1533,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1545,19 +1539,19 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AA2">
         <v>0</v>
       </c>
       <c r="AB2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC2">
         <v>1</v>
@@ -1569,13 +1563,13 @@
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AG2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1586,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1598,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1610,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1622,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1634,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1646,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y3">
         <v>1</v>
@@ -1658,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="AB3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -1670,84 +1664,84 @@
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -1759,25 +1753,25 @@
         <v>0</v>
       </c>
       <c r="AB4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AC4">
         <v>0</v>
       </c>
       <c r="AD4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AE4">
         <v>1</v>
       </c>
       <c r="AF4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AG4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1788,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1800,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1812,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1824,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1836,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1848,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -1860,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="AB5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -1872,36 +1866,36 @@
         <v>0</v>
       </c>
       <c r="AF5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AG5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1913,19 +1907,19 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1937,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1949,37 +1943,37 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AC6">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AE6">
         <v>0</v>
       </c>
       <c r="AF6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AG6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1990,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2002,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2014,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2026,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -2038,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -2050,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -2062,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="AB7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -2074,48 +2068,48 @@
         <v>0</v>
       </c>
       <c r="AF7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -2127,43 +2121,43 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AA8">
         <v>0</v>
       </c>
       <c r="AB8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -2175,48 +2169,48 @@
         <v>0</v>
       </c>
       <c r="AF8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AG8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -2228,7 +2222,7 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -2240,49 +2234,49 @@
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="W9">
         <v>1</v>
       </c>
       <c r="X9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y9">
         <v>1</v>
       </c>
       <c r="Z9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA9">
         <v>1</v>
       </c>
       <c r="AB9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AC9">
         <v>1</v>
       </c>
       <c r="AD9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE9">
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AG9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2293,7 +2287,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2305,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -2317,19 +2311,19 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2341,19 +2335,19 @@
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -2365,25 +2359,25 @@
         <v>0</v>
       </c>
       <c r="AB10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AE10">
         <v>1</v>
       </c>
       <c r="AF10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2394,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2406,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2418,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -2430,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2442,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -2454,19 +2448,19 @@
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
       <c r="AB11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -2478,13 +2472,13 @@
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AG11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2495,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2507,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2519,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -2531,7 +2525,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -2543,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -2555,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Y12">
         <v>0</v>
@@ -2567,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="AB12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -2579,13 +2573,13 @@
         <v>0</v>
       </c>
       <c r="AF12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AG12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2596,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2608,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -2620,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2632,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -2644,19 +2638,19 @@
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U13">
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Y13">
         <v>1</v>
@@ -2668,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="AB13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AC13">
         <v>0</v>
@@ -2680,13 +2674,13 @@
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AG13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2697,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2709,31 +2703,31 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -2745,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2757,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y14">
         <v>0</v>
@@ -2769,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="AB14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -2781,24 +2775,24 @@
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2810,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -2822,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2834,19 +2828,19 @@
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -2858,37 +2852,37 @@
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y15">
         <v>0</v>
       </c>
       <c r="Z15" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>285</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="s">
         <v>270</v>
       </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>271</v>
-      </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AG15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2899,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2911,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -2923,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2935,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -2947,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -2959,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -2971,48 +2965,48 @@
         <v>0</v>
       </c>
       <c r="AB16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AC16">
         <v>0</v>
       </c>
       <c r="AD16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AE16">
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AG16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -3024,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -3036,19 +3030,19 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S17">
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -3060,72 +3054,72 @@
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Y17">
         <v>0</v>
       </c>
       <c r="Z17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AA17">
         <v>0</v>
       </c>
       <c r="AB17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AC17">
         <v>0</v>
       </c>
       <c r="AD17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AE17">
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AG17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -3137,61 +3131,61 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S18">
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U18">
         <v>0</v>
       </c>
       <c r="V18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="W18">
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Y18">
         <v>0</v>
       </c>
       <c r="Z18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AA18">
         <v>0</v>
       </c>
       <c r="AB18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AG18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -3202,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -3214,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -3226,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -3238,19 +3232,19 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S19">
         <v>0</v>
       </c>
       <c r="T19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -3262,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Y19">
         <v>0</v>
@@ -3274,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="AB19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC19">
         <v>0</v>
@@ -3286,13 +3280,13 @@
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AG19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3303,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -3315,7 +3309,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -3327,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -3339,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -3351,7 +3345,7 @@
         <v>0</v>
       </c>
       <c r="T20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -3363,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Y20">
         <v>0</v>
@@ -3375,7 +3369,7 @@
         <v>1</v>
       </c>
       <c r="AB20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC20">
         <v>1</v>
@@ -3387,36 +3381,36 @@
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AG20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -3428,19 +3422,19 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -3452,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -3464,31 +3458,31 @@
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Y21">
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA21">
         <v>1</v>
       </c>
       <c r="AB21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AC21">
         <v>1</v>
       </c>
       <c r="AD21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AE21">
         <v>1</v>
       </c>
       <c r="AF21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AG21">
         <v>1</v>

</xml_diff>

<commit_message>
finished the correction in columns id for xcel files sup34
</commit_message>
<xml_diff>
--- a/data/figSup34Spk.xlsx
+++ b/data/figSup34Spk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdesbois/pg/chrisPg/centriG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033B6656-8A2B-BC49-ACCD-FCF2CE2520AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370CBCE7-515A-6549-BADF-BBC29B32A5A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,78 +90,6 @@
     <t>1649C_CXG4</t>
   </si>
   <si>
-    <t>vmscpIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>vmscfIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>vmscpCrossStcDlat50</t>
-  </si>
-  <si>
-    <t>vmscpIsoStcDgain50</t>
-  </si>
-  <si>
-    <t>vmscfIsoStcDgain50</t>
-  </si>
-  <si>
-    <t>vmscpCrossStcDgain50</t>
-  </si>
-  <si>
-    <t>vmscpIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmscfIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmscpCrossStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmscpIsoStcDgain50Indisig</t>
-  </si>
-  <si>
-    <t>vmscfIsoStcDgain50Indisig</t>
-  </si>
-  <si>
-    <t>vmscpCrossStcDgain50Indisig</t>
-  </si>
-  <si>
-    <t>vmfcpIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>vmfcpIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmfcpIsoStcDgain50</t>
-  </si>
-  <si>
-    <t>vmfcpIsoStcDgain50Indisig</t>
-  </si>
-  <si>
-    <t>vmfcfIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>vmfcfIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmfcfIsoStcDgain50</t>
-  </si>
-  <si>
-    <t>vmfcfIsoStcDgain50Indisig</t>
-  </si>
-  <si>
-    <t>vmfcpCrossStcDlat50</t>
-  </si>
-  <si>
-    <t>vmfcpCrossStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmfcpCrossStcDgain50</t>
-  </si>
-  <si>
-    <t>vmfcpCrossStcDgain50Indisig</t>
-  </si>
-  <si>
     <t>3.59999990463257E+0000</t>
   </si>
   <si>
@@ -342,24 +270,6 @@
     <t>4.09999990463257E+0000</t>
   </si>
   <si>
-    <t>vmsrndIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmsrndIsoStcDgain50</t>
-  </si>
-  <si>
-    <t>vmsrndIsoStcDgain50Indisig</t>
-  </si>
-  <si>
-    <t>vmfrndIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>vmfrndIsoStcDgain50</t>
-  </si>
-  <si>
-    <t>vmfrndIsoStcDgain50Indisig</t>
-  </si>
-  <si>
     <t>9.69999980926514E+0000</t>
   </si>
   <si>
@@ -984,10 +894,100 @@
     <t>5.20132362842560E-0001</t>
   </si>
   <si>
-    <t>vmsrndIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>vmfrndIsoStcDlat50</t>
+    <t>spkfrndIsoStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcDgain50</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcDlat50</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcDgain50</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcDlat50</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcDgain50</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcDlat50</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcDgain50</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcDlat50</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcDgain50</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcDlat50</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcDgain50</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcDlat50</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcDgain50</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcDlat50</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcDlat50Indisig</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcDgain50</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcDgain50Indisig</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcDlat50</t>
   </si>
 </sst>
 </file>
@@ -1372,100 +1372,100 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>292</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>293</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>294</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>295</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>296</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>297</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>298</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>299</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>300</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>301</v>
       </c>
       <c r="L1" t="s">
-        <v>25</v>
+        <v>302</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>303</v>
       </c>
       <c r="N1" t="s">
-        <v>37</v>
+        <v>304</v>
       </c>
       <c r="O1" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="P1" t="s">
-        <v>39</v>
+        <v>306</v>
       </c>
       <c r="Q1" t="s">
-        <v>40</v>
+        <v>307</v>
       </c>
       <c r="R1" t="s">
-        <v>23</v>
+        <v>308</v>
       </c>
       <c r="S1" t="s">
-        <v>29</v>
+        <v>309</v>
       </c>
       <c r="T1" t="s">
-        <v>26</v>
+        <v>310</v>
       </c>
       <c r="U1" t="s">
-        <v>32</v>
+        <v>311</v>
       </c>
       <c r="V1" t="s">
-        <v>41</v>
+        <v>312</v>
       </c>
       <c r="W1" t="s">
-        <v>42</v>
+        <v>313</v>
       </c>
       <c r="X1" t="s">
-        <v>43</v>
+        <v>314</v>
       </c>
       <c r="Y1" t="s">
-        <v>44</v>
+        <v>315</v>
       </c>
       <c r="Z1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AC1" t="s">
         <v>319</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>107</v>
       </c>
       <c r="AD1" t="s">
         <v>320</v>
       </c>
       <c r="AE1" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="AF1" t="s">
-        <v>109</v>
+        <v>290</v>
       </c>
       <c r="AG1" t="s">
-        <v>110</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -1473,97 +1473,97 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="W2">
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="AA2">
         <v>0</v>
       </c>
       <c r="AB2" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
       <c r="AC2">
         <v>1</v>
       </c>
       <c r="AD2" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>299</v>
+        <v>269</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -1574,97 +1574,97 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="U3">
         <v>1</v>
       </c>
       <c r="V3" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="W3">
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="AA3">
         <v>0</v>
       </c>
       <c r="AB3" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -1675,97 +1675,97 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>248</v>
+        <v>218</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="AA4">
         <v>0</v>
       </c>
       <c r="AB4" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="AC4">
         <v>0</v>
       </c>
       <c r="AD4" t="s">
-        <v>292</v>
+        <v>262</v>
       </c>
       <c r="AE4">
         <v>1</v>
       </c>
       <c r="AF4" t="s">
-        <v>301</v>
+        <v>271</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1776,97 +1776,97 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="AG5">
         <v>0</v>
@@ -1877,97 +1877,97 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6" t="s">
-        <v>276</v>
+        <v>246</v>
       </c>
       <c r="AC6">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="AE6">
         <v>0</v>
       </c>
       <c r="AF6" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -1978,97 +1978,97 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>251</v>
+        <v>221</v>
       </c>
       <c r="Y7">
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="AA7">
         <v>0</v>
       </c>
       <c r="AB7" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="AC7">
         <v>0</v>
       </c>
       <c r="AD7" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -2079,97 +2079,97 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>252</v>
+        <v>222</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="AA8">
         <v>0</v>
       </c>
       <c r="AB8" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="AC8">
         <v>0</v>
       </c>
       <c r="AD8" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="AG8">
         <v>0</v>
@@ -2180,97 +2180,97 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="W9">
         <v>1</v>
       </c>
       <c r="X9" t="s">
-        <v>253</v>
+        <v>223</v>
       </c>
       <c r="Y9">
         <v>1</v>
       </c>
       <c r="Z9" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="AA9">
         <v>1</v>
       </c>
       <c r="AB9" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
       <c r="AC9">
         <v>1</v>
       </c>
       <c r="AD9" t="s">
-        <v>294</v>
+        <v>264</v>
       </c>
       <c r="AE9">
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="AG9">
         <v>0</v>
@@ -2281,97 +2281,97 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="Y10">
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="AA10">
         <v>0</v>
       </c>
       <c r="AB10" t="s">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10" t="s">
-        <v>295</v>
+        <v>265</v>
       </c>
       <c r="AE10">
         <v>1</v>
       </c>
       <c r="AF10" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="AG10">
         <v>1</v>
@@ -2382,97 +2382,97 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
       <c r="AB11" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
       <c r="AC11">
         <v>0</v>
       </c>
       <c r="AD11" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="AE11">
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
       <c r="AG11">
         <v>0</v>
@@ -2483,97 +2483,97 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="U12">
         <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="W12">
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="Y12">
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="AA12">
         <v>0</v>
       </c>
       <c r="AB12" t="s">
-        <v>282</v>
+        <v>252</v>
       </c>
       <c r="AC12">
         <v>0</v>
       </c>
       <c r="AD12" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="AE12">
         <v>0</v>
       </c>
       <c r="AF12" t="s">
-        <v>309</v>
+        <v>279</v>
       </c>
       <c r="AG12">
         <v>0</v>
@@ -2584,97 +2584,97 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="U13">
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="Y13">
         <v>1</v>
       </c>
       <c r="Z13" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="AA13">
         <v>0</v>
       </c>
       <c r="AB13" t="s">
-        <v>283</v>
+        <v>253</v>
       </c>
       <c r="AC13">
         <v>0</v>
       </c>
       <c r="AD13" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="AE13">
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="AG13">
         <v>0</v>
@@ -2685,97 +2685,97 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="S14">
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="U14">
         <v>0</v>
       </c>
       <c r="V14" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="W14">
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="Y14">
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="AA14">
         <v>0</v>
       </c>
       <c r="AB14" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="AE14">
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>311</v>
+        <v>281</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -2786,97 +2786,97 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="U15">
         <v>0</v>
       </c>
       <c r="V15" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="Y15">
         <v>0</v>
       </c>
       <c r="Z15" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="AA15">
         <v>0</v>
       </c>
       <c r="AB15" t="s">
-        <v>285</v>
+        <v>255</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>312</v>
+        <v>282</v>
       </c>
       <c r="AG15">
         <v>0</v>
@@ -2887,97 +2887,97 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="S16">
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="U16">
         <v>0</v>
       </c>
       <c r="V16" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="Y16">
         <v>0</v>
       </c>
       <c r="Z16" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="AA16">
         <v>0</v>
       </c>
       <c r="AB16" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="AC16">
         <v>0</v>
       </c>
       <c r="AD16" t="s">
-        <v>296</v>
+        <v>266</v>
       </c>
       <c r="AE16">
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="AG16">
         <v>0</v>
@@ -2988,97 +2988,97 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="S17">
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="U17">
         <v>0</v>
       </c>
       <c r="V17" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="W17">
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="Y17">
         <v>0</v>
       </c>
       <c r="Z17" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="AA17">
         <v>0</v>
       </c>
       <c r="AB17" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="AC17">
         <v>0</v>
       </c>
       <c r="AD17" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="AE17">
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>314</v>
+        <v>284</v>
       </c>
       <c r="AG17">
         <v>0</v>
@@ -3089,97 +3089,97 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="S18">
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="U18">
         <v>0</v>
       </c>
       <c r="V18" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="W18">
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="Y18">
         <v>0</v>
       </c>
       <c r="Z18" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="AA18">
         <v>0</v>
       </c>
       <c r="AB18" t="s">
-        <v>288</v>
+        <v>258</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="AG18">
         <v>0</v>
@@ -3190,97 +3190,97 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="S19">
         <v>0</v>
       </c>
       <c r="T19" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="U19">
         <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="W19">
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
       <c r="Z19" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="AA19">
         <v>0</v>
       </c>
       <c r="AB19" t="s">
-        <v>289</v>
+        <v>259</v>
       </c>
       <c r="AC19">
         <v>0</v>
       </c>
       <c r="AD19" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="AE19">
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="AG19">
         <v>0</v>
@@ -3291,97 +3291,97 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="Q20">
         <v>0</v>
       </c>
       <c r="R20" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="U20">
         <v>0</v>
       </c>
       <c r="V20" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="W20">
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="Y20">
         <v>0</v>
       </c>
       <c r="Z20" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="AA20">
         <v>1</v>
       </c>
       <c r="AB20" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="AC20">
         <v>1</v>
       </c>
       <c r="AD20" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="AE20">
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
       <c r="AG20">
         <v>0</v>
@@ -3392,97 +3392,97 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>160</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
         <v>165</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>190</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" t="s">
-        <v>195</v>
-      </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="Q21">
         <v>0</v>
       </c>
       <c r="R21" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="S21">
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="U21">
         <v>0</v>
       </c>
       <c r="V21" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="W21">
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="Y21">
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="AA21">
         <v>1</v>
       </c>
       <c r="AB21" t="s">
-        <v>291</v>
+        <v>261</v>
       </c>
       <c r="AC21">
         <v>1</v>
       </c>
       <c r="AD21" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="AE21">
         <v>1</v>
       </c>
       <c r="AF21" t="s">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="AG21">
         <v>1</v>

</xml_diff>